<commit_message>
almost finished german translation
</commit_message>
<xml_diff>
--- a/strings_translsations_extractor/text.xlsx
+++ b/strings_translsations_extractor/text.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="10035" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="10035" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="4" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$B$2:$B$68</definedName>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="251">
   <si>
     <t>app_name</t>
   </si>
@@ -1157,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C74"/>
+    <sheetView topLeftCell="B48" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2414,7 +2415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B73"/>
     </sheetView>
   </sheetViews>
@@ -3007,4 +3008,607 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="2" max="2" width="85.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>